<commit_message>
se agrega la primera versión del cronograma en formato .xlsx
</commit_message>
<xml_diff>
--- a/Cronograma-v1.xlsx
+++ b/Cronograma-v1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Reibin\Trabajos\Tesis-Colegio\Documentos\documentos-6069Colegio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5E83959F-5582-4F96-8FD2-2A5A997451D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A73F922A-E264-4000-A723-8542B9921208}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{47A00661-3571-4181-A3BA-4AB20729DD3A}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="149">
   <si>
     <t>Trabajo</t>
   </si>
@@ -482,6 +482,9 @@
   </si>
   <si>
     <t>Fecha de inicio 20/12/2020</t>
+  </si>
+  <si>
+    <t>Cambio</t>
   </si>
 </sst>
 </file>
@@ -759,6 +762,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="4" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -789,25 +811,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Bueno" xfId="1" builtinId="26"/>
@@ -1176,7 +1179,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F832728-0D0A-4016-B1EB-6B174C9DD2A3}">
-  <dimension ref="A4:AD18"/>
+  <dimension ref="A4:AD19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
@@ -1283,9 +1286,9 @@
         <v>3210</v>
       </c>
     </row>
-    <row r="11" spans="1:30" s="41" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11"/>
-      <c r="B11" s="40" t="s">
+      <c r="B11" s="30" t="s">
         <v>15</v>
       </c>
       <c r="C11" s="14">
@@ -1357,11 +1360,11 @@
         <f>SUM(C6:C13)</f>
         <v>251</v>
       </c>
-      <c r="D14" s="33">
+      <c r="D14" s="23">
         <f>SUM(D6:D13)</f>
         <v>6840</v>
       </c>
-      <c r="E14" s="33">
+      <c r="E14" s="23">
         <f>SUM(E6:E13)</f>
         <v>7920</v>
       </c>
@@ -1380,6 +1383,11 @@
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>147</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -1611,7 +1619,7 @@
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B17" s="34" t="s">
+      <c r="B17" s="24" t="s">
         <v>145</v>
       </c>
       <c r="C17" s="2"/>
@@ -1877,14 +1885,14 @@
         <v>22</v>
       </c>
     </row>
-    <row r="41" spans="2:7" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="35" t="s">
+    <row r="41" spans="2:7" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="C41" s="36" t="s">
+      <c r="C41" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="D41" s="35"/>
+      <c r="D41" s="25"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B42" s="3" t="s">
@@ -1908,15 +1916,15 @@
         <v>22</v>
       </c>
     </row>
-    <row r="44" spans="2:7" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="35" t="s">
+    <row r="44" spans="2:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="C44" s="36" t="s">
+      <c r="C44" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="D44" s="36"/>
-      <c r="G44" s="39" t="s">
+      <c r="D44" s="26"/>
+      <c r="G44" s="29" t="s">
         <v>144</v>
       </c>
     </row>
@@ -1942,14 +1950,14 @@
         <v>21</v>
       </c>
     </row>
-    <row r="47" spans="2:7" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="36" t="s">
+    <row r="47" spans="2:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="C47" s="36" t="s">
+      <c r="C47" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="D47" s="36" t="s">
+      <c r="D47" s="26" t="s">
         <v>22</v>
       </c>
     </row>
@@ -2350,31 +2358,31 @@
   </cols>
   <sheetData>
     <row r="3" spans="6:19" x14ac:dyDescent="0.25">
-      <c r="G3" s="24" t="s">
+      <c r="G3" s="33" t="s">
         <v>93</v>
       </c>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="25" t="s">
+      <c r="H3" s="33"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25"/>
-      <c r="M3" s="26" t="s">
+      <c r="K3" s="34"/>
+      <c r="L3" s="34"/>
+      <c r="M3" s="35" t="s">
         <v>95</v>
       </c>
-      <c r="N3" s="26"/>
-      <c r="O3" s="26"/>
-      <c r="P3" s="28" t="s">
+      <c r="N3" s="35"/>
+      <c r="O3" s="35"/>
+      <c r="P3" s="37" t="s">
         <v>109</v>
       </c>
-      <c r="Q3" s="28" t="s">
+      <c r="Q3" s="37" t="s">
         <v>110</v>
       </c>
-      <c r="R3" s="28" t="s">
+      <c r="R3" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="S3" s="27" t="s">
+      <c r="S3" s="36" t="s">
         <v>108</v>
       </c>
     </row>
@@ -2409,10 +2417,10 @@
       <c r="O4" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="P4" s="28"/>
-      <c r="Q4" s="28"/>
-      <c r="R4" s="28"/>
-      <c r="S4" s="27"/>
+      <c r="P4" s="37"/>
+      <c r="Q4" s="37"/>
+      <c r="R4" s="37"/>
+      <c r="S4" s="36"/>
     </row>
     <row r="5" spans="6:19" x14ac:dyDescent="0.25">
       <c r="F5" s="6" t="s">
@@ -2497,11 +2505,11 @@
     </row>
     <row r="12" spans="6:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="6:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q13" s="23" t="s">
+      <c r="Q13" s="32" t="s">
         <v>112</v>
       </c>
-      <c r="R13" s="23"/>
-      <c r="S13" s="23"/>
+      <c r="R13" s="32"/>
+      <c r="S13" s="32"/>
     </row>
     <row r="14" spans="6:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -2533,16 +2541,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="6:20" x14ac:dyDescent="0.25">
-      <c r="H2" s="30" t="s">
+      <c r="H2" s="39" t="s">
         <v>115</v>
       </c>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="31" t="s">
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="40" t="s">
         <v>116</v>
       </c>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="40"/>
     </row>
     <row r="3" spans="6:20" x14ac:dyDescent="0.25">
       <c r="H3" t="s">
@@ -2622,81 +2630,81 @@
       </c>
     </row>
     <row r="17" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="E17" s="32" t="s">
+      <c r="E17" s="41" t="s">
         <v>127</v>
       </c>
-      <c r="G17" s="32" t="s">
+      <c r="G17" s="41" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="18" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="E18" s="32"/>
-      <c r="G18" s="32"/>
+      <c r="E18" s="41"/>
+      <c r="G18" s="41"/>
     </row>
     <row r="19" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="H19" s="32" t="s">
+      <c r="H19" s="41" t="s">
         <v>133</v>
       </c>
-      <c r="I19" s="32"/>
+      <c r="I19" s="41"/>
     </row>
     <row r="20" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="H20" s="32"/>
-      <c r="I20" s="32"/>
+      <c r="H20" s="41"/>
+      <c r="I20" s="41"/>
     </row>
     <row r="23" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D23" s="32" t="s">
+      <c r="D23" s="41" t="s">
         <v>132</v>
       </c>
-      <c r="F23" s="32" t="s">
+      <c r="F23" s="41" t="s">
         <v>131</v>
       </c>
-      <c r="H23" s="32" t="s">
+      <c r="H23" s="41" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="24" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D24" s="32"/>
-      <c r="F24" s="32"/>
-      <c r="H24" s="32"/>
+      <c r="D24" s="41"/>
+      <c r="F24" s="41"/>
+      <c r="H24" s="41"/>
     </row>
     <row r="25" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D25" s="32"/>
-      <c r="F25" s="32"/>
-      <c r="H25" s="32"/>
+      <c r="D25" s="41"/>
+      <c r="F25" s="41"/>
+      <c r="H25" s="41"/>
     </row>
     <row r="26" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D26" s="32"/>
-      <c r="F26" s="32"/>
-      <c r="H26" s="32"/>
+      <c r="D26" s="41"/>
+      <c r="F26" s="41"/>
+      <c r="H26" s="41"/>
     </row>
     <row r="27" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D27" s="32"/>
-      <c r="F27" s="32"/>
-      <c r="H27" s="32"/>
+      <c r="D27" s="41"/>
+      <c r="F27" s="41"/>
+      <c r="H27" s="41"/>
     </row>
     <row r="28" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D28" s="32"/>
-      <c r="F28" s="32"/>
-      <c r="H28" s="32"/>
+      <c r="D28" s="41"/>
+      <c r="F28" s="41"/>
+      <c r="H28" s="41"/>
     </row>
     <row r="29" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D29" s="32"/>
-      <c r="F29" s="32"/>
-      <c r="H29" s="32"/>
+      <c r="D29" s="41"/>
+      <c r="F29" s="41"/>
+      <c r="H29" s="41"/>
     </row>
     <row r="30" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D30" s="29"/>
-      <c r="E30" s="29"/>
-      <c r="F30" s="29"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
     </row>
     <row r="32" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D32" s="29" t="s">
+      <c r="D32" s="38" t="s">
         <v>135</v>
       </c>
-      <c r="E32" s="29"/>
-      <c r="F32" s="29"/>
-      <c r="G32" s="29"/>
-      <c r="H32" s="29"/>
+      <c r="E32" s="38"/>
+      <c r="F32" s="38"/>
+      <c r="G32" s="38"/>
+      <c r="H32" s="38"/>
     </row>
   </sheetData>
   <dataConsolidate/>

</xml_diff>